<commit_message>
fix bugs in some model fiels; null, blank
</commit_message>
<xml_diff>
--- a/data_excel/activity.xlsx
+++ b/data_excel/activity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\mini projects\AchReport\project\data_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\mini projects\AchReport01\project\data_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50C1E87-1100-4ABF-A037-8A61DD231A57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B174842-1A4E-452B-BD54-A030C1E744E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9996" xr2:uid="{B183BED3-8D9D-4C9D-91DB-3E99C66925F3}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="122">
   <si>
     <t>church</t>
   </si>
@@ -390,16 +390,10 @@
     <t>Womens Ministry</t>
   </si>
   <si>
-    <t>Ambassador</t>
-  </si>
-  <si>
-    <t>Pathfinder</t>
-  </si>
-  <si>
-    <t>Young Adult</t>
-  </si>
-  <si>
     <t>Congregation</t>
+  </si>
+  <si>
+    <t>Youth</t>
   </si>
 </sst>
 </file>
@@ -766,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D010DA14-FB87-4BEB-8C07-2CC237E35404}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -957,7 +951,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
@@ -1941,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>97</v>
@@ -1999,7 +1993,7 @@
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>101</v>
@@ -2028,7 +2022,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>103</v>

</xml_diff>